<commit_message>
refactor charts for report
</commit_message>
<xml_diff>
--- a/Analysis/calibration/factors_calibration/minions/30_repetitions_arrival_time_20sec/calibration_minion_response_time_arrival20sec.xlsx
+++ b/Analysis/calibration/factors_calibration/minions/30_repetitions_arrival_time_20sec/calibration_minion_response_time_arrival20sec.xlsx
@@ -368,7 +368,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -408,10 +408,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.113682040711157"/>
-          <c:y val="0.132753309466323"/>
-          <c:w val="0.857304818345787"/>
-          <c:h val="0.668137540587794"/>
+          <c:x val="0.113692561302287"/>
+          <c:y val="0.132711680959121"/>
+          <c:w val="0.857253245415207"/>
+          <c:h val="0.668054283573391"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1076,11 +1076,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25750518"/>
-        <c:axId val="91330357"/>
+        <c:axId val="45456364"/>
+        <c:axId val="12656170"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25750518"/>
+        <c:axId val="45456364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -1138,15 +1138,17 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91330357"/>
+        <c:crossAx val="12656170"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="2"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91330357"/>
+        <c:axId val="12656170"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="420"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1209,8 +1211,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25750518"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="45456364"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1268,9 +1270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>112680</xdr:colOff>
+      <xdr:colOff>112320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1278,8 +1280,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="38121480" y="2684520"/>
-        <a:ext cx="6985800" cy="4323960"/>
+        <a:off x="38130480" y="2684520"/>
+        <a:ext cx="6987960" cy="4323600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1299,11 +1301,11 @@
   </sheetPr>
   <dimension ref="B1:AB320"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V6" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF44" activeCellId="0" sqref="AF44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH44" activeCellId="0" sqref="AH44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.96"/>

</xml_diff>